<commit_message>
Modified Data Driven Test files
</commit_message>
<xml_diff>
--- a/DataTest/Data.xlsx
+++ b/DataTest/Data.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="Password">Sheet1!$B:$B</definedName>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="10">
   <si>
     <t>NataliaDamorad</t>
   </si>
@@ -41,6 +42,18 @@
   </si>
   <si>
     <t>qwerty12345000</t>
+  </si>
+  <si>
+    <t>EugenBorisik2</t>
+  </si>
+  <si>
+    <t>NataliaDamorad2</t>
+  </si>
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>Password</t>
   </si>
 </sst>
 </file>
@@ -93,6 +106,28 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Information" displayName="Information" ref="A1:B6" totalsRowShown="0">
+  <autoFilter ref="A1:B6"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="UserName"/>
+    <tableColumn id="2" name="Password"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Information2" displayName="Information2" ref="A1:B6" totalsRowShown="0">
+  <autoFilter ref="A1:B6"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="UserName"/>
+    <tableColumn id="2" name="Password"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -358,10 +393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -372,45 +407,126 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
         <v>4</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Modified files 6th Apr
</commit_message>
<xml_diff>
--- a/DataTest/Data.xlsx
+++ b/DataTest/Data.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="Password">Sheet1!$B:$B</definedName>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="10">
   <si>
     <t>NataliaDamorad</t>
   </si>
@@ -105,6 +106,28 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Information" displayName="Information" ref="A1:B6" totalsRowShown="0">
+  <autoFilter ref="A1:B6"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="UserName"/>
+    <tableColumn id="2" name="Password"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Information2" displayName="Information2" ref="A1:B6" totalsRowShown="0">
+  <autoFilter ref="A1:B6"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="UserName"/>
+    <tableColumn id="2" name="Password"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -372,8 +395,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -432,5 +455,78 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>